<commit_message>
refactor: add conditional formatting for order list
</commit_message>
<xml_diff>
--- a/docs/specification_python.xlsx
+++ b/docs/specification_python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yui00\src\prepare-to-pack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A50933-901F-46A4-94C1-BCA61B8A6ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED658312-25FC-41ED-A04A-9786C5F64154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Headers" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="205">
   <si>
     <t>Condition</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Target Column</t>
   </si>
   <si>
-    <t>fill red</t>
-  </si>
-  <si>
     <t>not null</t>
   </si>
   <si>
@@ -164,12 +161,6 @@
   </si>
   <si>
     <t>Cell Formatting</t>
-  </si>
-  <si>
-    <t>fill gray</t>
-  </si>
-  <si>
-    <t>fill blue</t>
   </si>
   <si>
     <t>Formatting</t>
@@ -855,6 +846,27 @@
   <si>
     <t>product_name</t>
   </si>
+  <si>
+    <t>iloc[0]</t>
+  </si>
+  <si>
+    <t>iloc</t>
+  </si>
+  <si>
+    <t>fill gray: RGB(190, 190, 190)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fill red: RGB(255, 204, 207) </t>
+  </si>
+  <si>
+    <t>fill blue: RGB(192, 230, 245)</t>
+  </si>
+  <si>
+    <t>ture</t>
+  </si>
+  <si>
+    <t>duplicate - 83, 135</t>
+  </si>
 </sst>
 </file>
 
@@ -902,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -924,6 +936,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1274,229 +1288,229 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1510,8 +1524,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1521,157 +1535,158 @@
     <col min="4" max="4" width="120.36328125" customWidth="1"/>
     <col min="5" max="5" width="30.1796875" customWidth="1"/>
     <col min="6" max="6" width="29.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" t="s">
-        <v>180</v>
-      </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4"/>
       <c r="D6" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4"/>
       <c r="D7" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4"/>
       <c r="D8" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="4"/>
       <c r="D9" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="4"/>
       <c r="D10" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" t="s">
         <v>142</v>
       </c>
-      <c r="C11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" t="s">
-        <v>145</v>
-      </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="8"/>
       <c r="E12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F13" s="2">
         <v>73</v>
@@ -1680,10 +1695,10 @@
     <row r="14" spans="1:6">
       <c r="B14" s="8"/>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F14" s="2">
         <v>194</v>
@@ -1692,10 +1707,10 @@
     <row r="15" spans="1:6">
       <c r="B15" s="8"/>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F15" s="2">
         <v>41</v>
@@ -1704,28 +1719,28 @@
     <row r="16" spans="1:6">
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F17" s="2">
         <v>104</v>
@@ -1734,7 +1749,7 @@
     <row r="18" spans="1:13">
       <c r="B18" s="8"/>
       <c r="E18" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2">
         <v>170</v>
@@ -1743,7 +1758,7 @@
     <row r="19" spans="1:13">
       <c r="B19" s="8"/>
       <c r="E19" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F19" s="2">
         <v>266</v>
@@ -1751,78 +1766,93 @@
     </row>
     <row r="20" spans="1:13">
       <c r="B20" s="8"/>
+      <c r="K20" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" t="s">
+        <v>197</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
         <v>72</v>
-      </c>
-      <c r="F22" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" t="s">
-        <v>200</v>
-      </c>
-      <c r="H22" t="s">
-        <v>70</v>
-      </c>
-      <c r="I22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="E24" t="s">
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
         <v>73</v>
       </c>
-      <c r="F24" t="s">
-        <v>76</v>
-      </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="E25" t="s">
-        <v>73</v>
+      <c r="D25" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H25">
         <v>4</v>
@@ -1830,90 +1860,104 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="3"/>
-      <c r="E26" t="s">
-        <v>80</v>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="E27" t="s">
-        <v>80</v>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="E28" t="s">
-        <v>83</v>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
     </row>
+    <row r="29" spans="1:13">
+      <c r="D29" t="s">
+        <v>204</v>
+      </c>
+    </row>
     <row r="30" spans="1:13">
       <c r="E30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="E31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="E32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H32">
         <v>3</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K32">
         <v>2</v>
       </c>
       <c r="L32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M32">
         <v>4</v>
@@ -1921,22 +1965,22 @@
     </row>
     <row r="33" spans="1:11">
       <c r="D33" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -1944,13 +1988,13 @@
     </row>
     <row r="34" spans="1:11">
       <c r="E34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1958,13 +2002,13 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1972,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1980,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1988,31 +2032,31 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="B39" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="B40" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="B41" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2020,12 +2064,12 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="C43" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2047,10 +2091,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="101" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2086,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2094,10 +2138,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -2111,10 +2155,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -2128,10 +2172,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2145,10 +2189,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -2162,10 +2206,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -2179,10 +2223,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -2196,10 +2240,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -2213,10 +2257,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -2230,10 +2274,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
@@ -2247,10 +2291,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>
@@ -2265,104 +2309,104 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F17">
         <v>1000</v>
@@ -2373,56 +2417,56 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20">
         <v>2.25</v>
@@ -2430,19 +2474,19 @@
     </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E21" t="s">
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2450,19 +2494,19 @@
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22">
         <v>8.1300000000000008</v>
@@ -2470,19 +2514,19 @@
     </row>
     <row r="23" spans="2:7">
       <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23">
         <v>6</v>
@@ -2490,19 +2534,19 @@
     </row>
     <row r="24" spans="2:7">
       <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
-        <v>36</v>
-      </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24">
         <v>30</v>
@@ -2510,19 +2554,19 @@
     </row>
     <row r="25" spans="2:7">
       <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25">
         <v>9</v>
@@ -2530,19 +2574,19 @@
     </row>
     <row r="26" spans="2:7">
       <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26">
         <v>3</v>
@@ -2550,19 +2594,19 @@
     </row>
     <row r="27" spans="2:7">
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27">
         <v>6</v>
@@ -2570,19 +2614,19 @@
     </row>
     <row r="28" spans="2:7">
       <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -2590,19 +2634,19 @@
     </row>
     <row r="29" spans="2:7">
       <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E29" t="s">
         <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2610,19 +2654,19 @@
     </row>
     <row r="30" spans="2:7">
       <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30">
         <v>8</v>
@@ -2630,19 +2674,19 @@
     </row>
     <row r="31" spans="2:7">
       <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E31" t="s">
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2650,19 +2694,19 @@
     </row>
     <row r="32" spans="2:7">
       <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G32">
         <v>29</v>
@@ -2670,19 +2714,19 @@
     </row>
     <row r="33" spans="2:7">
       <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E33" t="s">
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G33">
         <v>13</v>
@@ -2690,19 +2734,19 @@
     </row>
     <row r="34" spans="2:7">
       <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
         <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G34">
         <v>3.2</v>
@@ -2710,19 +2754,19 @@
     </row>
     <row r="35" spans="2:7">
       <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2730,19 +2774,19 @@
     </row>
     <row r="36" spans="2:7">
       <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
       <c r="D36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
         <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2750,222 +2794,222 @@
     </row>
     <row r="37" spans="2:7">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="2:7">
       <c r="B40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G40" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
         <v>27</v>
       </c>
       <c r="F41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G41" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s">
         <v>27</v>
       </c>
       <c r="F42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
         <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E44" t="s">
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:7">
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
         <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E47" t="s">
         <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Apply print and layout settings to order list file
</commit_message>
<xml_diff>
--- a/docs/specification_python.xlsx
+++ b/docs/specification_python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yui00\src\prepare-to-pack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED658312-25FC-41ED-A04A-9786C5F64154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941F15DC-1C81-47B5-A6B0-7F352C6625C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
+    <workbookView minimized="1" xWindow="6480" yWindow="-14955" windowWidth="14400" windowHeight="8175" xr2:uid="{48CDECB9-D0A6-43CF-B923-4C78336F5D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Headers" sheetId="6" r:id="rId1"/>
@@ -914,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -933,11 +933,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1275,7 +1274,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1581,7 +1580,7 @@
       <c r="A4" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>138</v>
       </c>
       <c r="C4" t="s">
@@ -1592,7 +1591,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>60</v>
       </c>
@@ -1652,7 +1651,7 @@
       <c r="A11" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>139</v>
       </c>
       <c r="C11" t="s">
@@ -1669,7 +1668,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="E12" t="s">
         <v>166</v>
       </c>
@@ -1678,7 +1677,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
       <c r="C13" t="s">
         <v>61</v>
       </c>
@@ -1693,7 +1692,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="8"/>
+      <c r="B14" s="9"/>
       <c r="D14" t="s">
         <v>180</v>
       </c>
@@ -1705,7 +1704,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="D15" t="s">
         <v>181</v>
       </c>
@@ -1717,7 +1716,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" t="s">
         <v>62</v>
       </c>
@@ -1732,7 +1731,7 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="B17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" t="s">
         <v>63</v>
       </c>
@@ -1747,7 +1746,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="B18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="E18" s="2" t="s">
         <v>146</v>
       </c>
@@ -1756,7 +1755,7 @@
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="B19" s="8"/>
+      <c r="B19" s="9"/>
       <c r="E19" s="2" t="s">
         <v>150</v>
       </c>
@@ -1765,7 +1764,7 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="B20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="K20" t="s">
         <v>198</v>
       </c>
@@ -1811,7 +1810,7 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F23" t="s">
@@ -1828,7 +1827,7 @@
       <c r="D24" t="b">
         <v>1</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F24" t="s">
@@ -1845,7 +1844,7 @@
       <c r="D25" t="s">
         <v>203</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" t="s">
         <v>70</v>
       </c>
       <c r="F25" t="s">
@@ -1863,7 +1862,7 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" t="s">
         <v>77</v>
       </c>
       <c r="F26" t="s">
@@ -1880,7 +1879,7 @@
       <c r="D27" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" t="s">
         <v>77</v>
       </c>
       <c r="F27" t="s">
@@ -1897,7 +1896,7 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" t="s">
         <v>80</v>
       </c>
       <c r="F28" t="s">
@@ -2091,10 +2090,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="C1" zoomScale="101" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>